<commit_message>
After completion of SearchAndSaveCastTest
</commit_message>
<xml_diff>
--- a/qaautomation.xlsx
+++ b/qaautomation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="162">
   <si>
     <t>Series Cast</t>
   </si>
@@ -510,6 +510,18 @@
   </si>
   <si>
     <t>Plastic Surgery Woman</t>
+  </si>
+  <si>
+    <t>Toby Foster</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>Julia Dearden</t>
+  </si>
+  <si>
+    <t>Nun</t>
   </si>
 </sst>
 </file>
@@ -925,7 +937,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1424,10 +1436,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1972,6 +1984,28 @@
         <v>117</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>

</xml_diff>